<commit_message>
Cleaned code and updated doe2 so it's clear that wt has 1 level.
</commit_message>
<xml_diff>
--- a/DOE2.xlsx
+++ b/DOE2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/000bbfc4ba40a858/phd/Models/Production planning with historical weather data/Reactor-Dash-App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DED8069-53BE-4E6F-8CDC-D87182F1C396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{3DED8069-53BE-4E6F-8CDC-D87182F1C396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD86C19E-9D6D-4185-AC86-F48A4CCFAFA8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B7D214A6-7DAF-4489-8D73-C889A1DFB1F9}"/>
   </bookViews>
@@ -407,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178C2A51-A2E5-47B3-8E6A-46E954B03CD1}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A74"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,7 +435,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -455,7 +455,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -515,7 +515,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -535,7 +535,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -555,7 +555,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -695,7 +695,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -775,7 +775,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -835,7 +835,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -895,7 +895,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -975,7 +975,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -1235,7 +1235,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1295,7 +1295,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1375,7 +1375,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -1455,7 +1455,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -1655,7 +1655,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -1695,7 +1695,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -1715,7 +1715,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -1815,7 +1815,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B74">
         <v>1</v>

</xml_diff>